<commit_message>
noch nicht alle fehler lt. review gelöst
</commit_message>
<xml_diff>
--- a/review_design_doc.xlsx
+++ b/review_design_doc.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="424">
   <si>
     <t>RID ID</t>
   </si>
@@ -833,7 +833,8 @@
     <t>Warum wird von "injizierten Fehlern" gesprochen? Können die Fehlertollereanzmechanismen etwa zwischen injizierten Fehlern und anderen Fehler unterscheiden?</t>
   </si>
   <si>
-    <t>wird nicht mehr gefunden im tex-file deswegen eh egal, zur klarstellung sei aber gesagt: die Fehler sind nunmal injiziert, alle nicht injizierten Fehler sind nicht von uns geplant und gehören hier also NICHT rein</t>
+    <t>klargestellt, dass auftredene fehler gemeint sind, die aber in diesem fall von uns absichlich injiziert werden
+</t>
   </si>
   <si>
     <t>FG-055</t>
@@ -1076,7 +1077,8 @@
     <t>Anmerkung: Inselbildung möglich je nach dem Auftrennen des Busses</t>
   </si>
   <si>
-    <t>tbd von der Gruppe</t>
+    <t>
+</t>
   </si>
   <si>
     <t>Fehler 6 </t>
@@ -1089,6 +1091,10 @@
   </si>
   <si>
     <t>Wie wird festgestellt, dass ein Abstandssensor ausgefallen ist?</t>
+  </si>
+  <si>
+    <t>
+was passiert, wenn fehlerhafte daten gesendet werden? vgl. kommentag im tex</t>
   </si>
   <si>
     <t>FG-074</t>
@@ -3839,7 +3845,7 @@
         <v>26</v>
       </c>
       <c t="s" s="11" r="H88">
-        <v>12</v>
+        <v>174</v>
       </c>
       <c s="4" r="I88"/>
     </row>
@@ -4504,7 +4510,7 @@
         <v>41</v>
       </c>
       <c t="s" s="3" r="H115">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c s="4" r="I115"/>
     </row>
@@ -4547,27 +4553,29 @@
         <v>357</v>
       </c>
       <c s="12" r="E117"/>
-      <c s="12" r="F117"/>
+      <c t="s" s="12" r="F117">
+        <v>358</v>
+      </c>
       <c t="s" s="7" r="G117">
         <v>11</v>
       </c>
       <c t="s" s="11" r="H117">
-        <v>12</v>
+        <v>224</v>
       </c>
       <c s="4" r="I117"/>
     </row>
     <row r="118">
       <c t="s" s="7" r="A118">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c t="s" s="8" r="B118">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c t="s" s="15" r="C118">
         <v>79</v>
       </c>
       <c t="s" s="15" r="D118">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c t="s" s="12" r="E118">
         <v>77</v>
@@ -4583,18 +4591,18 @@
     </row>
     <row customHeight="1" r="119" ht="45.0">
       <c t="s" s="7" r="A119">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" s="8" r="B119">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c s="15" r="C119"/>
       <c t="s" s="15" r="D119">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c s="12" r="E119"/>
       <c t="s" s="12" r="F119">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c t="s" s="7" r="G119">
         <v>26</v>
@@ -4606,14 +4614,14 @@
     </row>
     <row customHeight="1" r="120" ht="30.0">
       <c t="s" s="7" r="A120">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" s="8" r="B120">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c s="15" r="C120"/>
       <c t="s" s="15" r="D120">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c s="12" r="E120"/>
       <c s="12" r="F120"/>
@@ -4624,25 +4632,25 @@
         <v>12</v>
       </c>
       <c t="s" s="6" r="I120">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row customHeight="1" r="121" ht="45.0">
       <c t="s" s="7" r="A121">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" s="8" r="B121">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c t="s" s="15" r="C121">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c t="s" s="15" r="D121">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c s="12" r="E121"/>
       <c t="s" s="12" r="F121">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c t="s" s="7" r="G121">
         <v>11</v>
@@ -4654,20 +4662,20 @@
     </row>
     <row customHeight="1" r="122" ht="30.0">
       <c t="s" s="7" r="A122">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c t="s" s="8" r="B122">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c t="s" s="15" r="C122">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c t="s" s="15" r="D122">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c s="12" r="E122"/>
       <c t="s" s="12" r="F122">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c t="s" s="7" r="G122">
         <v>11</v>
@@ -4679,20 +4687,20 @@
     </row>
     <row customHeight="1" r="123" ht="30.0">
       <c t="s" s="7" r="A123">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c t="s" s="8" r="B123">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c t="s" s="15" r="C123">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c t="s" s="15" r="D123">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c s="12" r="E123"/>
       <c t="s" s="12" r="F123">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c t="s" s="7" r="G123">
         <v>11</v>
@@ -4704,20 +4712,20 @@
     </row>
     <row r="124">
       <c t="s" s="7" r="A124">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c t="s" s="8" r="B124">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c t="s" s="15" r="C124">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c t="s" s="15" r="D124">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c s="12" r="E124"/>
       <c t="s" s="12" r="F124">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c t="s" s="7" r="G124">
         <v>11</v>
@@ -4729,18 +4737,18 @@
     </row>
     <row r="125">
       <c t="s" s="7" r="A125">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c t="s" s="8" r="B125">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c s="15" r="C125"/>
       <c t="s" s="15" r="D125">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c s="12" r="E125"/>
       <c t="s" s="12" r="F125">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c t="s" s="7" r="G125">
         <v>11</v>
@@ -4752,16 +4760,16 @@
     </row>
     <row r="126">
       <c t="s" s="7" r="A126">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c t="s" s="8" r="B126">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c t="s" s="15" r="C126">
         <v>15</v>
       </c>
       <c t="s" s="15" r="D126">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c s="12" r="E126"/>
       <c s="12" r="F126"/>
@@ -4775,14 +4783,14 @@
     </row>
     <row customHeight="1" r="127" ht="30.0">
       <c t="s" s="7" r="A127">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c t="s" s="8" r="B127">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c s="15" r="C127"/>
       <c t="s" s="15" r="D127">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c s="12" r="E127"/>
       <c s="12" r="F127"/>
@@ -4793,19 +4801,19 @@
         <v>123</v>
       </c>
       <c t="s" s="6" r="I127">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row customHeight="1" r="128" ht="30.0">
       <c t="s" s="7" r="A128">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" s="8" r="B128">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c s="15" r="C128"/>
       <c t="s" s="15" r="D128">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c s="12" r="E128"/>
       <c s="12" r="F128"/>
@@ -4819,14 +4827,14 @@
     </row>
     <row customHeight="1" r="129" ht="30.0">
       <c t="s" s="7" r="A129">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c t="s" s="8" r="B129">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c s="15" r="C129"/>
       <c t="s" s="15" r="D129">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c s="12" r="E129"/>
       <c s="12" r="F129"/>
@@ -4840,14 +4848,14 @@
     </row>
     <row customHeight="1" r="130" ht="75.0">
       <c t="s" s="7" r="A130">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c t="s" s="8" r="B130">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c s="15" r="C130"/>
       <c t="s" s="15" r="D130">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c s="12" r="E130"/>
       <c s="12" r="F130"/>
@@ -4861,14 +4869,14 @@
     </row>
     <row r="131">
       <c t="s" s="7" r="A131">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c t="s" s="8" r="B131">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c s="15" r="C131"/>
       <c t="s" s="15" r="D131">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c s="12" r="E131"/>
       <c s="12" r="F131"/>
@@ -4882,20 +4890,20 @@
     </row>
     <row customHeight="1" r="132" ht="75.0">
       <c t="s" s="7" r="A132">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c t="s" s="8" r="B132">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c s="15" r="C132"/>
       <c t="s" s="15" r="D132">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c t="s" s="12" r="E132">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c t="s" s="12" r="F132">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c t="s" s="7" r="G132">
         <v>26</v>
@@ -4907,20 +4915,20 @@
     </row>
     <row r="133">
       <c t="s" s="7" r="A133">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c t="s" s="8" r="B133">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c s="15" r="C133"/>
       <c t="s" s="15" r="D133">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c t="s" s="12" r="E133">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c t="s" s="12" r="F133">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c t="s" s="7" r="G133">
         <v>11</v>
@@ -4932,17 +4940,17 @@
     </row>
     <row customHeight="1" r="134" ht="60.0">
       <c t="s" s="7" r="A134">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c t="s" s="8" r="B134">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c s="15" r="C134"/>
       <c t="s" s="15" r="D134">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c t="s" s="12" r="E134">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c s="12" r="F134"/>
       <c t="s" s="7" r="G134">
@@ -4955,17 +4963,17 @@
     </row>
     <row customHeight="1" r="135" ht="45.0">
       <c t="s" s="7" r="A135">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c t="s" s="8" r="B135">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c s="15" r="C135"/>
       <c t="s" s="15" r="D135">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c t="s" s="12" r="E135">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c s="12" r="F135"/>
       <c t="s" s="7" r="G135">
@@ -5391,7 +5399,7 @@
         <filter val="wie soll diese frage verstanden werden? Die beschreibung und der zweck dieses Diagramms sind direkt darunter erklärt (mit korrektem verweis)"/>
         <filter val="schriften angepasst wir empfehlen ausßerdem dieses seiten in anständiger qualität zu drucken"/>
         <filter val="wo am anfang besprochen? In diesem abschnitt? Einleitung dieses Abschnits schlanker gemacht so das die informationen mitsamt der graphischen veranschaulichung in der Aufzählung sind, komplett redundanten teil gekickt"/>
-        <filter val="wird nicht mehr gefunden im tex-file deswegen eh egal, zur klarstellung sei aber gesagt: die Fehler sind nunmal injiziert, alle nicht injizierten Fehler sind nicht von uns geplant und gehören hier also NICHT rein"/>
+        <filter val="klargestellt, dass auftredene fehler gemeint sind, die aber in diesem fall von uns absichlich injiziert werden "/>
         <filter val="ersetzt"/>
         <filter val="weg"/>
         <filter val="umformuliert"/>
@@ -5405,8 +5413,8 @@
         <filter val="Schwarz auf Hellblau"/>
         <filter val="nur die skalierung der Grafik ist anders, macht das sinn da irgendetwas zu ändern?"/>
         <filter val="nicht in unserem ausdruck"/>
-        <filter val="tbd von der Gruppe"/>
         <filter val="."/>
+        <filter val=" was passiert, wenn fehlerhafte daten gesendet werden? vgl. kommentag im tex"/>
         <filter val="verwiesen auf abb.7"/>
         <filter val="feiner aufgeöst in abbildung 13"/>
         <filter val="fehler werden über das ziehen von kabeln injiziert"/>
@@ -5416,6 +5424,8 @@
         <filter val="als großformatiges Ablaufdiagramm geplant, soll also groß sein, gehört auch NICHT auf eine A4 seite"/>
         <filter val="im gesamtausdruck ok"/>
         <filter val="tbd gruppe"/>
+        <filter val="wird nicht mehr gefunden im tex-file deswegen eh egal, zur klarstellung sei aber gesagt: die Fehler sind nunmal injiziert, alle nicht injizierten Fehler sind nicht von uns geplant und gehören hier also NICHT rein"/>
+        <filter val="tbd von der Gruppe"/>
       </filters>
     </filterColumn>
     <filterColumn colId="6">

</xml_diff>